<commit_message>
merged all changes from icwsm paper
</commit_message>
<xml_diff>
--- a/documentation/support_files/Final_Results.xlsx
+++ b/documentation/support_files/Final_Results.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" activeTab="1"/>
+    <workbookView xWindow="-80" yWindow="-440" windowWidth="25600" windowHeight="16000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Prediction_results" sheetId="11" r:id="rId1"/>
     <sheet name="Recall" sheetId="12" r:id="rId2"/>
     <sheet name="wordGrowth" sheetId="13" r:id="rId3"/>
     <sheet name="Pred. vs Time" sheetId="14" r:id="rId4"/>
+    <sheet name="HashTag Time Series" sheetId="15" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Election</t>
   </si>
@@ -92,6 +93,27 @@
   <si>
     <t>Chavez Vocabulary</t>
   </si>
+  <si>
+    <t>hashTag</t>
+  </si>
+  <si>
+    <t>beatles</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>elmundoconchavez</t>
+  </si>
+  <si>
+    <t>chavistas</t>
+  </si>
+  <si>
+    <t>ucvistasconchavez</t>
+  </si>
+  <si>
+    <t>vivachavez</t>
+  </si>
 </sst>
 </file>
 
@@ -100,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +161,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,7 +186,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -177,16 +206,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -196,6 +248,17 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -205,6 +268,17 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,11 +679,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2098847960"/>
-        <c:axId val="2098996760"/>
+        <c:axId val="2128824888"/>
+        <c:axId val="2128813608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2098847960"/>
+        <c:axId val="2128824888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,7 +692,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098996760"/>
+        <c:crossAx val="2128813608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -626,7 +700,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2098996760"/>
+        <c:axId val="2128813608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,21 +728,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098847960"/>
+        <c:crossAx val="2128824888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -713,7 +785,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -866,11 +937,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2091607384"/>
-        <c:axId val="2106133032"/>
+        <c:axId val="2128748344"/>
+        <c:axId val="2128742856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2091607384"/>
+        <c:axId val="2128748344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,13 +963,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106133032"/>
+        <c:crossAx val="2128742856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -906,7 +976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106133032"/>
+        <c:axId val="2128742856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -953,7 +1023,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091607384"/>
+        <c:crossAx val="2128748344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1014,7 +1084,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1246,11 +1315,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2088980536"/>
-        <c:axId val="2088986152"/>
+        <c:axId val="2128701560"/>
+        <c:axId val="2128695976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2088980536"/>
+        <c:axId val="2128701560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1276,14 +1345,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088986152"/>
+        <c:crossAx val="2128695976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1291,7 +1359,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2088986152"/>
+        <c:axId val="2128695976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,14 +1401,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088980536"/>
+        <c:crossAx val="2128701560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1507,11 +1574,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2089025496"/>
-        <c:axId val="2089028536"/>
+        <c:axId val="2128656648"/>
+        <c:axId val="2128653576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2089025496"/>
+        <c:axId val="2128656648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,7 +1588,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089028536"/>
+        <c:crossAx val="2128653576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1529,7 +1596,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089028536"/>
+        <c:axId val="2128653576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,14 +1607,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089025496"/>
+        <c:crossAx val="2128656648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2257,7 +2323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2623,4 +2689,260 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1">
+        <v>24</v>
+      </c>
+      <c r="C1">
+        <v>18</v>
+      </c>
+      <c r="D1">
+        <v>15</v>
+      </c>
+      <c r="E1">
+        <v>12</v>
+      </c>
+      <c r="F1">
+        <v>9</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>3</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>0.86956522802900005</v>
+      </c>
+      <c r="C2">
+        <v>0.86956522234</v>
+      </c>
+      <c r="D2">
+        <v>0.86956521974199996</v>
+      </c>
+      <c r="E2">
+        <v>0.86956521850699997</v>
+      </c>
+      <c r="F2">
+        <v>0.76512312000000005</v>
+      </c>
+      <c r="G2">
+        <v>0.81234119999999999</v>
+      </c>
+      <c r="H2">
+        <v>0.75123412000000001</v>
+      </c>
+      <c r="I2">
+        <v>0.79123421299999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.74474498239700004</v>
+      </c>
+      <c r="D3">
+        <v>0.36763937841900002</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>0.80032520618000003</v>
+      </c>
+      <c r="C4">
+        <v>0.69593496157800006</v>
+      </c>
+      <c r="D4">
+        <v>0.60516083007699994</v>
+      </c>
+      <c r="E4">
+        <v>0.52622680608500005</v>
+      </c>
+      <c r="F4">
+        <v>0.45758852640499997</v>
+      </c>
+      <c r="G4">
+        <v>0.56098323999999999</v>
+      </c>
+      <c r="H4">
+        <v>0.61324234</v>
+      </c>
+      <c r="I4">
+        <v>0.55231229999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>0.773297341995</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.78592625348599998</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0.37912323999999997</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.60129473282300006</v>
+      </c>
+      <c r="E6">
+        <v>0.52286498240299994</v>
+      </c>
+      <c r="F6">
+        <v>0.45466520146799999</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.36763937800000002</v>
+      </c>
+      <c r="H6">
+        <v>0.40233999999999998</v>
+      </c>
+      <c r="I6">
+        <v>0.38912311999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>0.62675629742500005</v>
+      </c>
+      <c r="C7">
+        <v>0.43595703799300001</v>
+      </c>
+      <c r="D7">
+        <v>0.34906271389499999</v>
+      </c>
+      <c r="E7">
+        <v>0.52027991832300002</v>
+      </c>
+      <c r="F7">
+        <v>0.45241874975800001</v>
+      </c>
+      <c r="G7">
+        <v>0.55231229999999998</v>
+      </c>
+      <c r="H7">
+        <v>0.69593496157800006</v>
+      </c>
+      <c r="I7">
+        <v>0.36763937841900002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.36323450000000002</v>
+      </c>
+      <c r="E8">
+        <v>0.45241874975800001</v>
+      </c>
+      <c r="F8">
+        <v>0.56098323999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.31323322999999997</v>
+      </c>
+      <c r="H8">
+        <v>0.61234124320000005</v>
+      </c>
+      <c r="I8">
+        <v>0.49912312399999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>